<commit_message>
add a STAR - check Dash characters in STAR
</commit_message>
<xml_diff>
--- a/trajectory/management/commands/SidStar/STAR-LFPG-LUKIP-08L.xlsx
+++ b/trajectory/management/commands/SidStar/STAR-LFPG-LUKIP-08L.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\git\flight-profile\trajectory\management\commands\SidStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C915DAF-8BEE-4AB6-AFA1-68219D69FB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945FBB23-9C74-4561-8622-5C44B822FB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E599D276-CC0B-4999-86A2-09540BAD0A64}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="19200" windowHeight="11170" xr2:uid="{E599D276-CC0B-4999-86A2-09540BAD0A64}"/>
   </bookViews>
   <sheets>
     <sheet name="WayPoints" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>order</t>
   </si>
@@ -92,9 +92,6 @@
     <t>CREPYENVALOIS</t>
   </si>
   <si>
-    <t>CROUYSUROURCQ</t>
-  </si>
-  <si>
     <t>N49°18'20.22"</t>
   </si>
   <si>
@@ -123,6 +120,24 @@
   </si>
   <si>
     <t>E003°04'27.80"</t>
+  </si>
+  <si>
+    <t>LIZY-SUR-OURCQ</t>
+  </si>
+  <si>
+    <t>CROUY-SUR-OURCQ</t>
+  </si>
+  <si>
+    <t>N49°01'06.00"</t>
+  </si>
+  <si>
+    <t>E003°01'00.00"</t>
+  </si>
+  <si>
+    <t>LA-FERTE-MILON</t>
+  </si>
+  <si>
+    <t>CREPY-EN-VALOIS</t>
   </si>
 </sst>
 </file>
@@ -474,19 +489,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3E1F7A-8251-4D41-A445-513320E03FDC}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.08984375" customWidth="1"/>
     <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.6328125" customWidth="1"/>
     <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -539,13 +554,16 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" t="s">
         <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -556,13 +574,16 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" t="s">
         <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -570,16 +591,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -587,16 +611,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -604,16 +631,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" t="s">
         <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -621,18 +651,38 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>